<commit_message>
Updated information on  work process followed
</commit_message>
<xml_diff>
--- a/Oswyn/Professional Work Process.xlsx
+++ b/Oswyn/Professional Work Process.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="0" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="1" r:id="rId1"/>
     <sheet name="Review Check List" sheetId="2" r:id="rId2"/>
     <sheet name="Release Checklist" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Professional Work Process</t>
   </si>
@@ -108,6 +108,160 @@
   </si>
   <si>
     <t xml:space="preserve">Verision </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Product  developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Legend 
+No go =&gt;  implies more work required cannot proceed , use '0' to indicate a no go situation
+ Go  =&gt; implies ready to go to next stage use '1' to indicate a situation where product development can proceed to next stage
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 hrs and above </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 hrs - 10 hrs </t>
+  </si>
+  <si>
+    <t>1. Document with new information requires revision change</t>
+  </si>
+  <si>
+    <t>7. Lessons learnt / Future Improvements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. stake holder meeting / expectation setting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Schedule </t>
+  </si>
+  <si>
+    <t>3. Budget /  Project cost control</t>
+  </si>
+  <si>
+    <t>5. Project risk / Mitigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Quality expectation /  Testing / document control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 hrs - 16 hrs </t>
+  </si>
+  <si>
+    <t>1. Use review checklist to ensure work for current stage  is complete</t>
+  </si>
+  <si>
+    <t>4. randome sample testing ( sample size 100)</t>
+  </si>
+  <si>
+    <t>2. prototype testing ,  software testing , functional test, system tests</t>
+  </si>
+  <si>
+    <t>3. randome sample testing  (sample size 10, ie 1 out of 10) + all above tests</t>
+  </si>
+  <si>
+    <t>Review , critique , feedback</t>
+  </si>
+  <si>
+    <t>Provide guidelines, liasion between client and project. 
+Define expectation, budget , schedule
+Highlight Risk
+Define standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. reviews </t>
+  </si>
+  <si>
+    <t>2. discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. decision making </t>
+  </si>
+  <si>
+    <t>2. meetings</t>
+  </si>
+  <si>
+    <t>1. For opinions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Information sharing </t>
+  </si>
+  <si>
+    <t>3. Informal project communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.  Formal request </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Formal Notification , reporting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. progress </t>
+  </si>
+  <si>
+    <t>1.meetings with respective stakeholders</t>
+  </si>
+  <si>
+    <t>3. Path forward</t>
+  </si>
+  <si>
+    <t>4. Agreement and effect of change on project</t>
+  </si>
+  <si>
+    <t>2. Risk evaluation, solution, options</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> resourses organization / team/ product design, development plan for standards, features , scalability , future features, new technology , existing technology / execution strategy</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2. work to proceed only after approval </t>
+  </si>
+  <si>
+    <t>5. Alignemt meetings with team, manager etc.</t>
+  </si>
+  <si>
+    <t>design, develop , maintain records &amp; documents , review , test assigned  product to manager based on set requirements by manager</t>
+  </si>
+  <si>
+    <t>1. organization of work ,  communicate expected requirements, workflow, meeting, discussions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. conferences meetings, discussion , reviews, </t>
+  </si>
+  <si>
+    <t>5. all other project communications</t>
   </si>
 </sst>
 </file>
@@ -120,6 +274,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,15 +308,27 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,8 +336,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,15 +378,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -217,6 +424,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -229,9 +437,51 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -558,121 +808,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="56.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="59.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="10" spans="1:7">
-      <c r="D10" t="s">
+      <c r="A10" s="11"/>
+      <c r="D10" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="G10" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11"/>
+      <c r="C11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" t="s">
+      <c r="A12" s="11"/>
+      <c r="E12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="F13" t="s">
+    <row r="13" spans="1:7" ht="14" customHeight="1">
+      <c r="A13" s="11"/>
+      <c r="C13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="5:6">
-      <c r="F18" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="5:6">
-      <c r="E19" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="5:6">
-      <c r="F22" t="s">
+      <c r="F19" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="E20" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="5:6">
-      <c r="F26" t="s">
+    <row r="23" spans="1:6">
+      <c r="F23" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="F24" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="F26" s="4" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="27" spans="1:6">
+      <c r="F27" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="F28" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="F29" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="F30" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="F31" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -685,48 +1097,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:11">
       <c r="A2" s="1"/>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="4" spans="1:11">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>B6+C6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D7:D18" si="0">B9+C9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G6:K12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6 D9 D12 D15 D18">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -742,7 +1294,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added professional work process and vector graphics
</commit_message>
<xml_diff>
--- a/Oswyn/Professional Work Process.xlsx
+++ b/Oswyn/Professional Work Process.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Professional Work Process</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">Verision </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name </t>
   </si>
   <si>
     <t xml:space="preserve">Version </t>
@@ -262,6 +259,15 @@
   </si>
   <si>
     <t>5. all other project communications</t>
+  </si>
+  <si>
+    <t>Oswyn's  WP-general</t>
+  </si>
+  <si>
+    <t>product definition document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Flow diagram </t>
   </si>
 </sst>
 </file>
@@ -352,8 +358,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,9 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -410,8 +415,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -425,6 +433,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -438,29 +447,10 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -810,272 +800,272 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="56.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="54.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="59.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="56.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="59.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>29</v>
+      <c r="B3" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="10"/>
+      <c r="D10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="10"/>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="10"/>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="C13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="F16" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="E19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="E20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="F22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="F23" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="F24" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="F26" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="F27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="5" t="s">
+    </row>
+    <row r="28" spans="1:6">
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="F29" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="F30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="11"/>
-      <c r="D10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="11"/>
-      <c r="C11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="11"/>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="C13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="E20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="F22" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="F23" s="5" t="s">
+    </row>
+    <row r="31" spans="1:6">
+      <c r="F31" s="4" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="F24" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="F26" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="F27" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="F28" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="F29" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="F30" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="F31" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1120,7 +1110,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1133,7 +1123,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1145,34 +1135,34 @@
         <f>B6+C6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="G6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1181,35 +1171,35 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D7:D18" si="0">B9+C9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+        <f t="shared" ref="D9:D18" si="0">B9+C9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1221,11 +1211,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
@@ -1234,7 +1224,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1254,7 +1244,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -1272,10 +1262,10 @@
     <mergeCell ref="G6:K12"/>
   </mergeCells>
   <conditionalFormatting sqref="D6 D9 D12 D15 D18">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1291,33 +1281,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1334,6 +1335,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>